<commit_message>
Updates to CSV extraction, new metadata for time stamps, better dynamic thresholding for stand-alone data.
</commit_message>
<xml_diff>
--- a/on_trucks/Processed_Stand_Alone/Median_Pulse_Widths_StandAlone.xlsx
+++ b/on_trucks/Processed_Stand_Alone/Median_Pulse_Widths_StandAlone.xlsx
@@ -666,7 +666,7 @@
         <v>0.5</v>
       </c>
       <c r="C2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>47</v>
@@ -695,7 +695,7 @@
         <v>0.7</v>
       </c>
       <c r="C3">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>47</v>
@@ -724,7 +724,7 @@
         <v>0.8</v>
       </c>
       <c r="C4">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4">
         <v>47</v>
@@ -753,7 +753,7 @@
         <v>0.9</v>
       </c>
       <c r="C5">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5">
         <v>47</v>
@@ -782,7 +782,7 @@
         <v>0.5</v>
       </c>
       <c r="C6">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>39</v>
@@ -811,7 +811,7 @@
         <v>0.7</v>
       </c>
       <c r="C7">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>39</v>
@@ -869,7 +869,7 @@
         <v>0.9</v>
       </c>
       <c r="C9">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9">
         <v>39</v>
@@ -927,7 +927,7 @@
         <v>0.7</v>
       </c>
       <c r="C11">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11">
         <v>14</v>
@@ -956,7 +956,7 @@
         <v>0.8</v>
       </c>
       <c r="C12">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12">
         <v>14</v>
@@ -985,7 +985,7 @@
         <v>0.9</v>
       </c>
       <c r="C13">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13">
         <v>14</v>
@@ -1043,7 +1043,7 @@
         <v>0.7</v>
       </c>
       <c r="C15">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15">
         <v>48</v>
@@ -1072,7 +1072,7 @@
         <v>0.8</v>
       </c>
       <c r="C16">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16">
         <v>48</v>
@@ -1101,7 +1101,7 @@
         <v>0.9</v>
       </c>
       <c r="C17">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17">
         <v>48</v>
@@ -1130,7 +1130,7 @@
         <v>0.5</v>
       </c>
       <c r="C18">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>40</v>
@@ -1159,7 +1159,7 @@
         <v>0.7</v>
       </c>
       <c r="C19">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19">
         <v>40</v>
@@ -1188,7 +1188,7 @@
         <v>0.8</v>
       </c>
       <c r="C20">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20">
         <v>40</v>
@@ -1275,7 +1275,7 @@
         <v>0.7</v>
       </c>
       <c r="C23">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23">
         <v>54</v>
@@ -1362,7 +1362,7 @@
         <v>0.5</v>
       </c>
       <c r="C26">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26">
         <v>61</v>
@@ -1391,7 +1391,7 @@
         <v>0.7</v>
       </c>
       <c r="C27">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D27">
         <v>61</v>
@@ -1420,7 +1420,7 @@
         <v>0.8</v>
       </c>
       <c r="C28">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D28">
         <v>61</v>
@@ -1449,7 +1449,7 @@
         <v>0.9</v>
       </c>
       <c r="C29">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D29">
         <v>61</v>
@@ -1478,7 +1478,7 @@
         <v>0.5</v>
       </c>
       <c r="C30">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30">
         <v>59</v>
@@ -1507,7 +1507,7 @@
         <v>0.7</v>
       </c>
       <c r="C31">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D31">
         <v>59</v>
@@ -1536,7 +1536,7 @@
         <v>0.8</v>
       </c>
       <c r="C32">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32">
         <v>59</v>
@@ -1565,7 +1565,7 @@
         <v>0.9</v>
       </c>
       <c r="C33">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33">
         <v>59</v>
@@ -1594,7 +1594,7 @@
         <v>0.5</v>
       </c>
       <c r="C34">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D34">
         <v>56</v>
@@ -1623,7 +1623,7 @@
         <v>0.7</v>
       </c>
       <c r="C35">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D35">
         <v>56</v>
@@ -1681,7 +1681,7 @@
         <v>0.9</v>
       </c>
       <c r="C37">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D37">
         <v>56</v>
@@ -1710,7 +1710,7 @@
         <v>0.5</v>
       </c>
       <c r="C38">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D38">
         <v>58</v>
@@ -1739,7 +1739,7 @@
         <v>0.7</v>
       </c>
       <c r="C39">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D39">
         <v>58</v>
@@ -1768,7 +1768,7 @@
         <v>0.8</v>
       </c>
       <c r="C40">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D40">
         <v>58</v>
@@ -1797,7 +1797,7 @@
         <v>0.9</v>
       </c>
       <c r="C41">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D41">
         <v>58</v>
@@ -1826,7 +1826,7 @@
         <v>0.5</v>
       </c>
       <c r="C42">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D42">
         <v>12</v>
@@ -1855,7 +1855,7 @@
         <v>0.7</v>
       </c>
       <c r="C43">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D43">
         <v>12</v>
@@ -1884,7 +1884,7 @@
         <v>0.8</v>
       </c>
       <c r="C44">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D44">
         <v>12</v>
@@ -1913,7 +1913,7 @@
         <v>0.9</v>
       </c>
       <c r="C45">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D45">
         <v>12</v>
@@ -1971,7 +1971,7 @@
         <v>0.7</v>
       </c>
       <c r="C47">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D47">
         <v>22</v>
@@ -2029,7 +2029,7 @@
         <v>0.9</v>
       </c>
       <c r="C49">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D49">
         <v>22</v>
@@ -2058,7 +2058,7 @@
         <v>0.5</v>
       </c>
       <c r="C50">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D50">
         <v>28</v>
@@ -2087,7 +2087,7 @@
         <v>0.7</v>
       </c>
       <c r="C51">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D51">
         <v>28</v>
@@ -2116,7 +2116,7 @@
         <v>0.8</v>
       </c>
       <c r="C52">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D52">
         <v>28</v>
@@ -2145,7 +2145,7 @@
         <v>0.9</v>
       </c>
       <c r="C53">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D53">
         <v>28</v>
@@ -2203,7 +2203,7 @@
         <v>0.7</v>
       </c>
       <c r="C55">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D55">
         <v>3</v>
@@ -2261,7 +2261,7 @@
         <v>0.9</v>
       </c>
       <c r="C57">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D57">
         <v>3</v>
@@ -2290,7 +2290,7 @@
         <v>0.5</v>
       </c>
       <c r="C58">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D58">
         <v>49</v>
@@ -2319,7 +2319,7 @@
         <v>0.7</v>
       </c>
       <c r="C59">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D59">
         <v>49</v>
@@ -2348,7 +2348,7 @@
         <v>0.8</v>
       </c>
       <c r="C60">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="D60">
         <v>49</v>
@@ -2377,7 +2377,7 @@
         <v>0.9</v>
       </c>
       <c r="C61">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="D61">
         <v>49</v>
@@ -2406,7 +2406,7 @@
         <v>0.5</v>
       </c>
       <c r="C62">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D62">
         <v>27</v>
@@ -2435,7 +2435,7 @@
         <v>0.7</v>
       </c>
       <c r="C63">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D63">
         <v>27</v>
@@ -2464,7 +2464,7 @@
         <v>0.8</v>
       </c>
       <c r="C64">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D64">
         <v>27</v>
@@ -2493,7 +2493,7 @@
         <v>0.9</v>
       </c>
       <c r="C65">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D65">
         <v>27</v>
@@ -2522,7 +2522,7 @@
         <v>0.5</v>
       </c>
       <c r="C66">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D66">
         <v>24</v>
@@ -2551,7 +2551,7 @@
         <v>0.7</v>
       </c>
       <c r="C67">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D67">
         <v>24</v>
@@ -2580,7 +2580,7 @@
         <v>0.8</v>
       </c>
       <c r="C68">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D68">
         <v>24</v>
@@ -2609,7 +2609,7 @@
         <v>0.9</v>
       </c>
       <c r="C69">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D69">
         <v>24</v>
@@ -2638,7 +2638,7 @@
         <v>0.5</v>
       </c>
       <c r="C70">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D70">
         <v>17</v>
@@ -2667,7 +2667,7 @@
         <v>0.7</v>
       </c>
       <c r="C71">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D71">
         <v>17</v>
@@ -2696,7 +2696,7 @@
         <v>0.8</v>
       </c>
       <c r="C72">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D72">
         <v>17</v>
@@ -2725,7 +2725,7 @@
         <v>0.9</v>
       </c>
       <c r="C73">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D73">
         <v>17</v>
@@ -2783,7 +2783,7 @@
         <v>0.7</v>
       </c>
       <c r="C75">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D75">
         <v>19</v>
@@ -2870,7 +2870,7 @@
         <v>0.5</v>
       </c>
       <c r="C78">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D78">
         <v>34</v>
@@ -2928,7 +2928,7 @@
         <v>0.8</v>
       </c>
       <c r="C80">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D80">
         <v>34</v>
@@ -2957,7 +2957,7 @@
         <v>0.9</v>
       </c>
       <c r="C81">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D81">
         <v>34</v>
@@ -2986,7 +2986,7 @@
         <v>0.5</v>
       </c>
       <c r="C82">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D82">
         <v>30</v>
@@ -3015,7 +3015,7 @@
         <v>0.7</v>
       </c>
       <c r="C83">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D83">
         <v>30</v>
@@ -3044,7 +3044,7 @@
         <v>0.8</v>
       </c>
       <c r="C84">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D84">
         <v>30</v>
@@ -3073,7 +3073,7 @@
         <v>0.9</v>
       </c>
       <c r="C85">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D85">
         <v>30</v>
@@ -3102,7 +3102,7 @@
         <v>0.5</v>
       </c>
       <c r="C86">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D86">
         <v>50</v>
@@ -3131,7 +3131,7 @@
         <v>0.7</v>
       </c>
       <c r="C87">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D87">
         <v>50</v>
@@ -3160,7 +3160,7 @@
         <v>0.8</v>
       </c>
       <c r="C88">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D88">
         <v>50</v>
@@ -3189,7 +3189,7 @@
         <v>0.9</v>
       </c>
       <c r="C89">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D89">
         <v>50</v>
@@ -3218,7 +3218,7 @@
         <v>0.5</v>
       </c>
       <c r="C90">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D90">
         <v>10</v>
@@ -3247,7 +3247,7 @@
         <v>0.7</v>
       </c>
       <c r="C91">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D91">
         <v>10</v>
@@ -3276,7 +3276,7 @@
         <v>0.8</v>
       </c>
       <c r="C92">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D92">
         <v>10</v>
@@ -3305,7 +3305,7 @@
         <v>0.9</v>
       </c>
       <c r="C93">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D93">
         <v>10</v>
@@ -3363,7 +3363,7 @@
         <v>0.7</v>
       </c>
       <c r="C95">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D95">
         <v>60</v>
@@ -3392,7 +3392,7 @@
         <v>0.8</v>
       </c>
       <c r="C96">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D96">
         <v>60</v>
@@ -3421,7 +3421,7 @@
         <v>0.9</v>
       </c>
       <c r="C97">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D97">
         <v>60</v>
@@ -3450,7 +3450,7 @@
         <v>0.5</v>
       </c>
       <c r="C98">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -3479,7 +3479,7 @@
         <v>0.7</v>
       </c>
       <c r="C99">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -3508,7 +3508,7 @@
         <v>0.8</v>
       </c>
       <c r="C100">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -3537,7 +3537,7 @@
         <v>0.9</v>
       </c>
       <c r="C101">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -3566,7 +3566,7 @@
         <v>0.5</v>
       </c>
       <c r="C102">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D102">
         <v>51</v>
@@ -3595,7 +3595,7 @@
         <v>0.7</v>
       </c>
       <c r="C103">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D103">
         <v>51</v>
@@ -3624,7 +3624,7 @@
         <v>0.8</v>
       </c>
       <c r="C104">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D104">
         <v>51</v>
@@ -3653,7 +3653,7 @@
         <v>0.9</v>
       </c>
       <c r="C105">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D105">
         <v>51</v>
@@ -3798,7 +3798,7 @@
         <v>0.5</v>
       </c>
       <c r="C110">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D110">
         <v>5</v>
@@ -3827,7 +3827,7 @@
         <v>0.7</v>
       </c>
       <c r="C111">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D111">
         <v>5</v>
@@ -3885,7 +3885,7 @@
         <v>0.9</v>
       </c>
       <c r="C113">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D113">
         <v>5</v>
@@ -3914,7 +3914,7 @@
         <v>0.5</v>
       </c>
       <c r="C114">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D114">
         <v>63</v>
@@ -3943,7 +3943,7 @@
         <v>0.7</v>
       </c>
       <c r="C115">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D115">
         <v>63</v>
@@ -3972,7 +3972,7 @@
         <v>0.8</v>
       </c>
       <c r="C116">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D116">
         <v>63</v>
@@ -4001,7 +4001,7 @@
         <v>0.9</v>
       </c>
       <c r="C117">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D117">
         <v>63</v>
@@ -4030,7 +4030,7 @@
         <v>0.5</v>
       </c>
       <c r="C118">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D118">
         <v>7</v>
@@ -4059,7 +4059,7 @@
         <v>0.7</v>
       </c>
       <c r="C119">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D119">
         <v>7</v>
@@ -4146,7 +4146,7 @@
         <v>0.5</v>
       </c>
       <c r="C122">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D122">
         <v>52</v>
@@ -4175,7 +4175,7 @@
         <v>0.7</v>
       </c>
       <c r="C123">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D123">
         <v>52</v>
@@ -4204,7 +4204,7 @@
         <v>0.8</v>
       </c>
       <c r="C124">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D124">
         <v>52</v>
@@ -4233,7 +4233,7 @@
         <v>0.9</v>
       </c>
       <c r="C125">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D125">
         <v>52</v>
@@ -4262,7 +4262,7 @@
         <v>0.5</v>
       </c>
       <c r="C126">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D126">
         <v>16</v>
@@ -4291,7 +4291,7 @@
         <v>0.7</v>
       </c>
       <c r="C127">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D127">
         <v>16</v>
@@ -4320,7 +4320,7 @@
         <v>0.8</v>
       </c>
       <c r="C128">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D128">
         <v>16</v>
@@ -4349,7 +4349,7 @@
         <v>0.9</v>
       </c>
       <c r="C129">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D129">
         <v>16</v>
@@ -4378,7 +4378,7 @@
         <v>0.5</v>
       </c>
       <c r="C130">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D130">
         <v>46</v>
@@ -4407,7 +4407,7 @@
         <v>0.7</v>
       </c>
       <c r="C131">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D131">
         <v>46</v>
@@ -4436,7 +4436,7 @@
         <v>0.8</v>
       </c>
       <c r="C132">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D132">
         <v>46</v>
@@ -4465,7 +4465,7 @@
         <v>0.9</v>
       </c>
       <c r="C133">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D133">
         <v>46</v>
@@ -4523,7 +4523,7 @@
         <v>0.7</v>
       </c>
       <c r="C135">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D135">
         <v>55</v>
@@ -4552,7 +4552,7 @@
         <v>0.8</v>
       </c>
       <c r="C136">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D136">
         <v>55</v>
@@ -4610,7 +4610,7 @@
         <v>0.5</v>
       </c>
       <c r="C138">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D138">
         <v>6</v>
@@ -4639,7 +4639,7 @@
         <v>0.7</v>
       </c>
       <c r="C139">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D139">
         <v>6</v>
@@ -4726,7 +4726,7 @@
         <v>0.5</v>
       </c>
       <c r="C142">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D142">
         <v>45</v>
@@ -4755,7 +4755,7 @@
         <v>0.7</v>
       </c>
       <c r="C143">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D143">
         <v>45</v>
@@ -4784,7 +4784,7 @@
         <v>0.8</v>
       </c>
       <c r="C144">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D144">
         <v>45</v>
@@ -4813,7 +4813,7 @@
         <v>0.9</v>
       </c>
       <c r="C145">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D145">
         <v>45</v>
@@ -4842,7 +4842,7 @@
         <v>0.5</v>
       </c>
       <c r="C146">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D146">
         <v>4</v>
@@ -4958,7 +4958,7 @@
         <v>0.5</v>
       </c>
       <c r="C150">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D150">
         <v>44</v>
@@ -4987,7 +4987,7 @@
         <v>0.7</v>
       </c>
       <c r="C151">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D151">
         <v>44</v>
@@ -5016,7 +5016,7 @@
         <v>0.8</v>
       </c>
       <c r="C152">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D152">
         <v>44</v>
@@ -5045,7 +5045,7 @@
         <v>0.9</v>
       </c>
       <c r="C153">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D153">
         <v>44</v>
@@ -5074,7 +5074,7 @@
         <v>0.5</v>
       </c>
       <c r="C154">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D154">
         <v>38</v>
@@ -5132,7 +5132,7 @@
         <v>0.8</v>
       </c>
       <c r="C156">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D156">
         <v>38</v>
@@ -5161,7 +5161,7 @@
         <v>0.9</v>
       </c>
       <c r="C157">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D157">
         <v>38</v>
@@ -5190,7 +5190,7 @@
         <v>0.5</v>
       </c>
       <c r="C158">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D158">
         <v>13</v>
@@ -5219,7 +5219,7 @@
         <v>0.7</v>
       </c>
       <c r="C159">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D159">
         <v>13</v>
@@ -5248,7 +5248,7 @@
         <v>0.8</v>
       </c>
       <c r="C160">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D160">
         <v>13</v>
@@ -5306,7 +5306,7 @@
         <v>0.5</v>
       </c>
       <c r="C162">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D162">
         <v>20</v>
@@ -5335,7 +5335,7 @@
         <v>0.7</v>
       </c>
       <c r="C163">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D163">
         <v>20</v>
@@ -5364,7 +5364,7 @@
         <v>0.8</v>
       </c>
       <c r="C164">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D164">
         <v>20</v>
@@ -5451,7 +5451,7 @@
         <v>0.7</v>
       </c>
       <c r="C167">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D167">
         <v>18</v>
@@ -5480,7 +5480,7 @@
         <v>0.8</v>
       </c>
       <c r="C168">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D168">
         <v>18</v>
@@ -5509,7 +5509,7 @@
         <v>0.9</v>
       </c>
       <c r="C169">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D169">
         <v>18</v>
@@ -5567,7 +5567,7 @@
         <v>0.7</v>
       </c>
       <c r="C171">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D171">
         <v>11</v>
@@ -5596,7 +5596,7 @@
         <v>0.8</v>
       </c>
       <c r="C172">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D172">
         <v>11</v>
@@ -5625,7 +5625,7 @@
         <v>0.9</v>
       </c>
       <c r="C173">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D173">
         <v>11</v>
@@ -5654,7 +5654,7 @@
         <v>0.5</v>
       </c>
       <c r="C174">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D174">
         <v>57</v>
@@ -5683,7 +5683,7 @@
         <v>0.7</v>
       </c>
       <c r="C175">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D175">
         <v>57</v>
@@ -5712,7 +5712,7 @@
         <v>0.8</v>
       </c>
       <c r="C176">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D176">
         <v>57</v>
@@ -5741,7 +5741,7 @@
         <v>0.9</v>
       </c>
       <c r="C177">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D177">
         <v>57</v>
@@ -5770,7 +5770,7 @@
         <v>0.5</v>
       </c>
       <c r="C178">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D178">
         <v>32</v>
@@ -5828,7 +5828,7 @@
         <v>0.8</v>
       </c>
       <c r="C180">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D180">
         <v>32</v>
@@ -5857,7 +5857,7 @@
         <v>0.9</v>
       </c>
       <c r="C181">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D181">
         <v>32</v>
@@ -5915,7 +5915,7 @@
         <v>0.7</v>
       </c>
       <c r="C183">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D183">
         <v>62</v>
@@ -5944,7 +5944,7 @@
         <v>0.8</v>
       </c>
       <c r="C184">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D184">
         <v>62</v>
@@ -6002,7 +6002,7 @@
         <v>0.5</v>
       </c>
       <c r="C186">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D186">
         <v>36</v>
@@ -6031,7 +6031,7 @@
         <v>0.7</v>
       </c>
       <c r="C187">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D187">
         <v>36</v>
@@ -6060,7 +6060,7 @@
         <v>0.8</v>
       </c>
       <c r="C188">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D188">
         <v>36</v>
@@ -6089,7 +6089,7 @@
         <v>0.9</v>
       </c>
       <c r="C189">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D189">
         <v>36</v>
@@ -6147,7 +6147,7 @@
         <v>0.7</v>
       </c>
       <c r="C191">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D191">
         <v>23</v>
@@ -6176,7 +6176,7 @@
         <v>0.8</v>
       </c>
       <c r="C192">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D192">
         <v>23</v>
@@ -6205,7 +6205,7 @@
         <v>0.9</v>
       </c>
       <c r="C193">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D193">
         <v>23</v>
@@ -6234,7 +6234,7 @@
         <v>0.5</v>
       </c>
       <c r="C194">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D194">
         <v>42</v>
@@ -6263,7 +6263,7 @@
         <v>0.7</v>
       </c>
       <c r="C195">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D195">
         <v>42</v>
@@ -6292,7 +6292,7 @@
         <v>0.8</v>
       </c>
       <c r="C196">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D196">
         <v>42</v>
@@ -6321,7 +6321,7 @@
         <v>0.9</v>
       </c>
       <c r="C197">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D197">
         <v>42</v>
@@ -6350,7 +6350,7 @@
         <v>0.5</v>
       </c>
       <c r="C198">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D198">
         <v>2</v>
@@ -6379,7 +6379,7 @@
         <v>0.7</v>
       </c>
       <c r="C199">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D199">
         <v>2</v>
@@ -6408,7 +6408,7 @@
         <v>0.8</v>
       </c>
       <c r="C200">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D200">
         <v>2</v>
@@ -6437,7 +6437,7 @@
         <v>0.9</v>
       </c>
       <c r="C201">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D201">
         <v>2</v>
@@ -6466,7 +6466,7 @@
         <v>0.5</v>
       </c>
       <c r="C202">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D202">
         <v>26</v>
@@ -6524,7 +6524,7 @@
         <v>0.8</v>
       </c>
       <c r="C204">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D204">
         <v>26</v>
@@ -6553,7 +6553,7 @@
         <v>0.9</v>
       </c>
       <c r="C205">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D205">
         <v>26</v>
@@ -6582,7 +6582,7 @@
         <v>0.5</v>
       </c>
       <c r="C206">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D206">
         <v>15</v>
@@ -6611,7 +6611,7 @@
         <v>0.7</v>
       </c>
       <c r="C207">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D207">
         <v>15</v>
@@ -6640,7 +6640,7 @@
         <v>0.8</v>
       </c>
       <c r="C208">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D208">
         <v>15</v>
@@ -6669,7 +6669,7 @@
         <v>0.9</v>
       </c>
       <c r="C209">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D209">
         <v>15</v>
@@ -6698,7 +6698,7 @@
         <v>0.5</v>
       </c>
       <c r="C210">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D210">
         <v>31</v>
@@ -6727,7 +6727,7 @@
         <v>0.7</v>
       </c>
       <c r="C211">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D211">
         <v>31</v>
@@ -6756,7 +6756,7 @@
         <v>0.8</v>
       </c>
       <c r="C212">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D212">
         <v>31</v>
@@ -6785,7 +6785,7 @@
         <v>0.9</v>
       </c>
       <c r="C213">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D213">
         <v>31</v>
@@ -6814,7 +6814,7 @@
         <v>0.5</v>
       </c>
       <c r="C214">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D214">
         <v>21</v>
@@ -6843,7 +6843,7 @@
         <v>0.7</v>
       </c>
       <c r="C215">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D215">
         <v>21</v>
@@ -6872,7 +6872,7 @@
         <v>0.8</v>
       </c>
       <c r="C216">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D216">
         <v>21</v>
@@ -6901,7 +6901,7 @@
         <v>0.9</v>
       </c>
       <c r="C217">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D217">
         <v>21</v>
@@ -6930,7 +6930,7 @@
         <v>0.5</v>
       </c>
       <c r="C218">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D218">
         <v>53</v>
@@ -6959,7 +6959,7 @@
         <v>0.7</v>
       </c>
       <c r="C219">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D219">
         <v>53</v>
@@ -6988,7 +6988,7 @@
         <v>0.8</v>
       </c>
       <c r="C220">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="D220">
         <v>53</v>
@@ -7017,7 +7017,7 @@
         <v>0.9</v>
       </c>
       <c r="C221">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="D221">
         <v>53</v>
@@ -7046,7 +7046,7 @@
         <v>0.5</v>
       </c>
       <c r="C222">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D222">
         <v>8</v>
@@ -7075,7 +7075,7 @@
         <v>0.7</v>
       </c>
       <c r="C223">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D223">
         <v>8</v>
@@ -7104,7 +7104,7 @@
         <v>0.8</v>
       </c>
       <c r="C224">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D224">
         <v>8</v>
@@ -7133,7 +7133,7 @@
         <v>0.9</v>
       </c>
       <c r="C225">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D225">
         <v>8</v>
@@ -7162,7 +7162,7 @@
         <v>0.5</v>
       </c>
       <c r="C226">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D226">
         <v>35</v>
@@ -7191,7 +7191,7 @@
         <v>0.7</v>
       </c>
       <c r="C227">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D227">
         <v>35</v>
@@ -7220,7 +7220,7 @@
         <v>0.8</v>
       </c>
       <c r="C228">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D228">
         <v>35</v>
@@ -7249,7 +7249,7 @@
         <v>0.9</v>
       </c>
       <c r="C229">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D229">
         <v>35</v>
@@ -7278,7 +7278,7 @@
         <v>0.5</v>
       </c>
       <c r="C230">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D230">
         <v>43</v>
@@ -7307,7 +7307,7 @@
         <v>0.7</v>
       </c>
       <c r="C231">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D231">
         <v>43</v>
@@ -7336,7 +7336,7 @@
         <v>0.8</v>
       </c>
       <c r="C232">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D232">
         <v>43</v>
@@ -7365,7 +7365,7 @@
         <v>0.9</v>
       </c>
       <c r="C233">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D233">
         <v>43</v>

</xml_diff>

<commit_message>
Added Fixed Baseline Subtraction method to pulse_width_calculator.py
</commit_message>
<xml_diff>
--- a/on_trucks/Processed_Stand_Alone/Median_Pulse_Widths_StandAlone.xlsx
+++ b/on_trucks/Processed_Stand_Alone/Median_Pulse_Widths_StandAlone.xlsx
@@ -840,7 +840,7 @@
         <v>0.5</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>67</v>
@@ -869,7 +869,7 @@
         <v>0.7</v>
       </c>
       <c r="C3">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>67</v>
@@ -898,7 +898,7 @@
         <v>0.8</v>
       </c>
       <c r="C4">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>67</v>
@@ -927,7 +927,7 @@
         <v>0.9</v>
       </c>
       <c r="C5">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
         <v>67</v>
@@ -956,7 +956,7 @@
         <v>0.5</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>68</v>
@@ -985,7 +985,7 @@
         <v>0.7</v>
       </c>
       <c r="C7">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>68</v>
@@ -1014,7 +1014,7 @@
         <v>0.8</v>
       </c>
       <c r="C8">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>68</v>
@@ -1043,7 +1043,7 @@
         <v>0.9</v>
       </c>
       <c r="C9">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -1072,7 +1072,7 @@
         <v>0.5</v>
       </c>
       <c r="C10">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
         <v>69</v>
@@ -1101,7 +1101,7 @@
         <v>0.7</v>
       </c>
       <c r="C11">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
         <v>69</v>
@@ -1130,7 +1130,7 @@
         <v>0.8</v>
       </c>
       <c r="C12">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>69</v>
@@ -1159,7 +1159,7 @@
         <v>0.9</v>
       </c>
       <c r="C13">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
         <v>69</v>
@@ -1188,7 +1188,7 @@
         <v>0.5</v>
       </c>
       <c r="C14">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
         <v>70</v>
@@ -1217,7 +1217,7 @@
         <v>0.7</v>
       </c>
       <c r="C15">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
         <v>70</v>
@@ -1246,7 +1246,7 @@
         <v>0.8</v>
       </c>
       <c r="C16">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
         <v>70</v>
@@ -1275,7 +1275,7 @@
         <v>0.9</v>
       </c>
       <c r="C17">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
         <v>70</v>
@@ -1304,7 +1304,7 @@
         <v>0.5</v>
       </c>
       <c r="C18">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
         <v>71</v>
@@ -1333,7 +1333,7 @@
         <v>0.7</v>
       </c>
       <c r="C19">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
         <v>71</v>
@@ -1362,7 +1362,7 @@
         <v>0.8</v>
       </c>
       <c r="C20">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
         <v>71</v>
@@ -1391,7 +1391,7 @@
         <v>0.9</v>
       </c>
       <c r="C21">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
         <v>71</v>
@@ -1420,7 +1420,7 @@
         <v>0.5</v>
       </c>
       <c r="C22">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
         <v>72</v>
@@ -1449,7 +1449,7 @@
         <v>0.7</v>
       </c>
       <c r="C23">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
         <v>72</v>
@@ -1478,7 +1478,7 @@
         <v>0.8</v>
       </c>
       <c r="C24">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="D24" t="s">
         <v>72</v>
@@ -1507,7 +1507,7 @@
         <v>0.9</v>
       </c>
       <c r="C25">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
         <v>72</v>
@@ -1536,7 +1536,7 @@
         <v>0.5</v>
       </c>
       <c r="C26">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
         <v>73</v>
@@ -1565,7 +1565,7 @@
         <v>0.7</v>
       </c>
       <c r="C27">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
         <v>73</v>
@@ -1594,7 +1594,7 @@
         <v>0.8</v>
       </c>
       <c r="C28">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
         <v>73</v>
@@ -1623,7 +1623,7 @@
         <v>0.9</v>
       </c>
       <c r="C29">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
         <v>73</v>
@@ -1652,7 +1652,7 @@
         <v>0.5</v>
       </c>
       <c r="C30">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
         <v>74</v>
@@ -1681,7 +1681,7 @@
         <v>0.7</v>
       </c>
       <c r="C31">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D31" t="s">
         <v>74</v>
@@ -1710,7 +1710,7 @@
         <v>0.8</v>
       </c>
       <c r="C32">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s">
         <v>74</v>
@@ -1739,7 +1739,7 @@
         <v>0.9</v>
       </c>
       <c r="C33">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D33" t="s">
         <v>74</v>
@@ -1768,7 +1768,7 @@
         <v>0.5</v>
       </c>
       <c r="C34">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D34" t="s">
         <v>75</v>
@@ -1797,7 +1797,7 @@
         <v>0.7</v>
       </c>
       <c r="C35">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
         <v>75</v>
@@ -1826,7 +1826,7 @@
         <v>0.8</v>
       </c>
       <c r="C36">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="D36" t="s">
         <v>75</v>
@@ -1855,7 +1855,7 @@
         <v>0.9</v>
       </c>
       <c r="C37">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
         <v>75</v>
@@ -1913,7 +1913,7 @@
         <v>0.7</v>
       </c>
       <c r="C39">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D39" t="s">
         <v>76</v>
@@ -1942,7 +1942,7 @@
         <v>0.8</v>
       </c>
       <c r="C40">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
         <v>76</v>
@@ -1971,7 +1971,7 @@
         <v>0.9</v>
       </c>
       <c r="C41">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
         <v>76</v>
@@ -2000,7 +2000,7 @@
         <v>0.5</v>
       </c>
       <c r="C42">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
         <v>77</v>
@@ -2029,7 +2029,7 @@
         <v>0.7</v>
       </c>
       <c r="C43">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="D43" t="s">
         <v>77</v>
@@ -2058,7 +2058,7 @@
         <v>0.8</v>
       </c>
       <c r="C44">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
         <v>77</v>
@@ -2087,7 +2087,7 @@
         <v>0.9</v>
       </c>
       <c r="C45">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="D45" t="s">
         <v>77</v>
@@ -2116,7 +2116,7 @@
         <v>0.5</v>
       </c>
       <c r="C46">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D46" t="s">
         <v>78</v>
@@ -2145,7 +2145,7 @@
         <v>0.7</v>
       </c>
       <c r="C47">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D47" t="s">
         <v>78</v>
@@ -2174,7 +2174,7 @@
         <v>0.8</v>
       </c>
       <c r="C48">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="D48" t="s">
         <v>78</v>
@@ -2203,7 +2203,7 @@
         <v>0.9</v>
       </c>
       <c r="C49">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="D49" t="s">
         <v>78</v>
@@ -2232,7 +2232,7 @@
         <v>0.5</v>
       </c>
       <c r="C50">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="D50" t="s">
         <v>79</v>
@@ -2261,7 +2261,7 @@
         <v>0.7</v>
       </c>
       <c r="C51">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="D51" t="s">
         <v>79</v>
@@ -2290,7 +2290,7 @@
         <v>0.8</v>
       </c>
       <c r="C52">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="D52" t="s">
         <v>79</v>
@@ -2319,7 +2319,7 @@
         <v>0.9</v>
       </c>
       <c r="C53">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="D53" t="s">
         <v>79</v>
@@ -2348,7 +2348,7 @@
         <v>0.5</v>
       </c>
       <c r="C54">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D54" t="s">
         <v>80</v>
@@ -2377,7 +2377,7 @@
         <v>0.7</v>
       </c>
       <c r="C55">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D55" t="s">
         <v>80</v>
@@ -2406,7 +2406,7 @@
         <v>0.8</v>
       </c>
       <c r="C56">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="D56" t="s">
         <v>80</v>
@@ -2435,7 +2435,7 @@
         <v>0.9</v>
       </c>
       <c r="C57">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="D57" t="s">
         <v>80</v>
@@ -2464,7 +2464,7 @@
         <v>0.5</v>
       </c>
       <c r="C58">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D58" t="s">
         <v>81</v>
@@ -2493,7 +2493,7 @@
         <v>0.7</v>
       </c>
       <c r="C59">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D59" t="s">
         <v>81</v>
@@ -2522,7 +2522,7 @@
         <v>0.8</v>
       </c>
       <c r="C60">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D60" t="s">
         <v>81</v>
@@ -2551,7 +2551,7 @@
         <v>0.9</v>
       </c>
       <c r="C61">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="D61" t="s">
         <v>81</v>
@@ -2580,7 +2580,7 @@
         <v>0.5</v>
       </c>
       <c r="C62">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="D62" t="s">
         <v>82</v>
@@ -2638,7 +2638,7 @@
         <v>0.8</v>
       </c>
       <c r="C64">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D64" t="s">
         <v>82</v>
@@ -2667,7 +2667,7 @@
         <v>0.9</v>
       </c>
       <c r="C65">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="D65" t="s">
         <v>82</v>
@@ -2696,7 +2696,7 @@
         <v>0.5</v>
       </c>
       <c r="C66">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D66" t="s">
         <v>83</v>
@@ -2725,7 +2725,7 @@
         <v>0.7</v>
       </c>
       <c r="C67">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="D67" t="s">
         <v>83</v>
@@ -2754,7 +2754,7 @@
         <v>0.8</v>
       </c>
       <c r="C68">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="D68" t="s">
         <v>83</v>
@@ -2783,7 +2783,7 @@
         <v>0.9</v>
       </c>
       <c r="C69">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="D69" t="s">
         <v>83</v>
@@ -2812,7 +2812,7 @@
         <v>0.5</v>
       </c>
       <c r="C70">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D70" t="s">
         <v>84</v>
@@ -2841,7 +2841,7 @@
         <v>0.7</v>
       </c>
       <c r="C71">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D71" t="s">
         <v>84</v>
@@ -2870,7 +2870,7 @@
         <v>0.8</v>
       </c>
       <c r="C72">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D72" t="s">
         <v>84</v>
@@ -2899,7 +2899,7 @@
         <v>0.9</v>
       </c>
       <c r="C73">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="D73" t="s">
         <v>84</v>
@@ -2928,7 +2928,7 @@
         <v>0.5</v>
       </c>
       <c r="C74">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="D74" t="s">
         <v>85</v>
@@ -2957,7 +2957,7 @@
         <v>0.7</v>
       </c>
       <c r="C75">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="D75" t="s">
         <v>85</v>
@@ -2986,7 +2986,7 @@
         <v>0.8</v>
       </c>
       <c r="C76">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D76" t="s">
         <v>85</v>
@@ -3015,7 +3015,7 @@
         <v>0.9</v>
       </c>
       <c r="C77">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="D77" t="s">
         <v>85</v>
@@ -3044,7 +3044,7 @@
         <v>0.5</v>
       </c>
       <c r="C78">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D78" t="s">
         <v>86</v>
@@ -3073,7 +3073,7 @@
         <v>0.7</v>
       </c>
       <c r="C79">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D79" t="s">
         <v>86</v>
@@ -3102,7 +3102,7 @@
         <v>0.8</v>
       </c>
       <c r="C80">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="D80" t="s">
         <v>86</v>
@@ -3131,7 +3131,7 @@
         <v>0.9</v>
       </c>
       <c r="C81">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="D81" t="s">
         <v>86</v>
@@ -3160,7 +3160,7 @@
         <v>0.5</v>
       </c>
       <c r="C82">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D82" t="s">
         <v>87</v>
@@ -3189,7 +3189,7 @@
         <v>0.7</v>
       </c>
       <c r="C83">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D83" t="s">
         <v>87</v>
@@ -3218,7 +3218,7 @@
         <v>0.8</v>
       </c>
       <c r="C84">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="D84" t="s">
         <v>87</v>
@@ -3247,7 +3247,7 @@
         <v>0.9</v>
       </c>
       <c r="C85">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -3276,7 +3276,7 @@
         <v>0.5</v>
       </c>
       <c r="C86">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -3305,7 +3305,7 @@
         <v>0.7</v>
       </c>
       <c r="C87">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="D87" t="s">
         <v>88</v>
@@ -3334,7 +3334,7 @@
         <v>0.8</v>
       </c>
       <c r="C88">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D88" t="s">
         <v>88</v>
@@ -3363,7 +3363,7 @@
         <v>0.9</v>
       </c>
       <c r="C89">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="D89" t="s">
         <v>88</v>
@@ -3392,7 +3392,7 @@
         <v>0.5</v>
       </c>
       <c r="C90">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D90" t="s">
         <v>89</v>
@@ -3421,7 +3421,7 @@
         <v>0.7</v>
       </c>
       <c r="C91">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="D91" t="s">
         <v>89</v>
@@ -3450,7 +3450,7 @@
         <v>0.8</v>
       </c>
       <c r="C92">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D92" t="s">
         <v>89</v>
@@ -3479,7 +3479,7 @@
         <v>0.9</v>
       </c>
       <c r="C93">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D93" t="s">
         <v>89</v>
@@ -3508,7 +3508,7 @@
         <v>0.5</v>
       </c>
       <c r="C94">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D94" t="s">
         <v>90</v>
@@ -3537,7 +3537,7 @@
         <v>0.7</v>
       </c>
       <c r="C95">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D95" t="s">
         <v>90</v>
@@ -3566,7 +3566,7 @@
         <v>0.8</v>
       </c>
       <c r="C96">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="D96" t="s">
         <v>90</v>
@@ -3595,7 +3595,7 @@
         <v>0.9</v>
       </c>
       <c r="C97">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="D97" t="s">
         <v>90</v>
@@ -3624,7 +3624,7 @@
         <v>0.5</v>
       </c>
       <c r="C98">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D98" t="s">
         <v>91</v>
@@ -3653,7 +3653,7 @@
         <v>0.7</v>
       </c>
       <c r="C99">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D99" t="s">
         <v>91</v>
@@ -3682,7 +3682,7 @@
         <v>0.8</v>
       </c>
       <c r="C100">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="D100" t="s">
         <v>91</v>
@@ -3711,7 +3711,7 @@
         <v>0.9</v>
       </c>
       <c r="C101">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D101" t="s">
         <v>91</v>
@@ -3740,7 +3740,7 @@
         <v>0.5</v>
       </c>
       <c r="C102">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D102" t="s">
         <v>92</v>
@@ -3769,7 +3769,7 @@
         <v>0.7</v>
       </c>
       <c r="C103">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D103" t="s">
         <v>92</v>
@@ -3798,7 +3798,7 @@
         <v>0.8</v>
       </c>
       <c r="C104">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="D104" t="s">
         <v>92</v>
@@ -3827,7 +3827,7 @@
         <v>0.9</v>
       </c>
       <c r="C105">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="D105" t="s">
         <v>92</v>
@@ -3856,7 +3856,7 @@
         <v>0.5</v>
       </c>
       <c r="C106">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D106" t="s">
         <v>93</v>
@@ -3885,7 +3885,7 @@
         <v>0.7</v>
       </c>
       <c r="C107">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="D107" t="s">
         <v>93</v>
@@ -3914,7 +3914,7 @@
         <v>0.8</v>
       </c>
       <c r="C108">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="D108" t="s">
         <v>93</v>
@@ -3943,7 +3943,7 @@
         <v>0.9</v>
       </c>
       <c r="C109">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D109" t="s">
         <v>93</v>
@@ -3972,7 +3972,7 @@
         <v>0.5</v>
       </c>
       <c r="C110">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D110" t="s">
         <v>94</v>
@@ -4001,7 +4001,7 @@
         <v>0.7</v>
       </c>
       <c r="C111">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="D111" t="s">
         <v>94</v>
@@ -4030,7 +4030,7 @@
         <v>0.8</v>
       </c>
       <c r="C112">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="D112" t="s">
         <v>94</v>
@@ -4059,7 +4059,7 @@
         <v>0.9</v>
       </c>
       <c r="C113">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D113" t="s">
         <v>94</v>
@@ -4088,7 +4088,7 @@
         <v>0.5</v>
       </c>
       <c r="C114">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D114" t="s">
         <v>95</v>
@@ -4117,7 +4117,7 @@
         <v>0.7</v>
       </c>
       <c r="C115">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D115" t="s">
         <v>95</v>
@@ -4146,7 +4146,7 @@
         <v>0.8</v>
       </c>
       <c r="C116">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="D116" t="s">
         <v>95</v>
@@ -4175,7 +4175,7 @@
         <v>0.9</v>
       </c>
       <c r="C117">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="D117" t="s">
         <v>95</v>
@@ -4204,7 +4204,7 @@
         <v>0.5</v>
       </c>
       <c r="C118">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D118" t="s">
         <v>96</v>
@@ -4233,7 +4233,7 @@
         <v>0.7</v>
       </c>
       <c r="C119">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="D119" t="s">
         <v>96</v>
@@ -4262,7 +4262,7 @@
         <v>0.8</v>
       </c>
       <c r="C120">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="D120" t="s">
         <v>96</v>
@@ -4291,7 +4291,7 @@
         <v>0.9</v>
       </c>
       <c r="C121">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="D121" t="s">
         <v>96</v>
@@ -4320,7 +4320,7 @@
         <v>0.5</v>
       </c>
       <c r="C122">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="D122" t="s">
         <v>97</v>
@@ -4349,7 +4349,7 @@
         <v>0.7</v>
       </c>
       <c r="C123">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="D123" t="s">
         <v>97</v>
@@ -4378,7 +4378,7 @@
         <v>0.8</v>
       </c>
       <c r="C124">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="D124" t="s">
         <v>97</v>
@@ -4407,7 +4407,7 @@
         <v>0.9</v>
       </c>
       <c r="C125">
-        <v>129</v>
+        <v>60</v>
       </c>
       <c r="D125" t="s">
         <v>97</v>
@@ -4436,7 +4436,7 @@
         <v>0.5</v>
       </c>
       <c r="C126">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="D126" t="s">
         <v>98</v>
@@ -4465,7 +4465,7 @@
         <v>0.7</v>
       </c>
       <c r="C127">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="D127" t="s">
         <v>98</v>
@@ -4494,7 +4494,7 @@
         <v>0.8</v>
       </c>
       <c r="C128">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="D128" t="s">
         <v>98</v>
@@ -4523,7 +4523,7 @@
         <v>0.9</v>
       </c>
       <c r="C129">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="D129" t="s">
         <v>98</v>
@@ -4552,7 +4552,7 @@
         <v>0.5</v>
       </c>
       <c r="C130">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="D130" t="s">
         <v>99</v>
@@ -4581,7 +4581,7 @@
         <v>0.7</v>
       </c>
       <c r="C131">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="D131" t="s">
         <v>99</v>
@@ -4610,7 +4610,7 @@
         <v>0.8</v>
       </c>
       <c r="C132">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="D132" t="s">
         <v>99</v>
@@ -4639,7 +4639,7 @@
         <v>0.9</v>
       </c>
       <c r="C133">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="D133" t="s">
         <v>99</v>
@@ -4668,7 +4668,7 @@
         <v>0.5</v>
       </c>
       <c r="C134">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D134" t="s">
         <v>100</v>
@@ -4697,7 +4697,7 @@
         <v>0.7</v>
       </c>
       <c r="C135">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D135" t="s">
         <v>100</v>
@@ -4726,7 +4726,7 @@
         <v>0.8</v>
       </c>
       <c r="C136">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D136" t="s">
         <v>100</v>
@@ -4755,7 +4755,7 @@
         <v>0.9</v>
       </c>
       <c r="C137">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D137" t="s">
         <v>100</v>
@@ -4784,7 +4784,7 @@
         <v>0.5</v>
       </c>
       <c r="C138">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="D138" t="s">
         <v>101</v>
@@ -4813,7 +4813,7 @@
         <v>0.7</v>
       </c>
       <c r="C139">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="D139" t="s">
         <v>101</v>
@@ -4842,7 +4842,7 @@
         <v>0.8</v>
       </c>
       <c r="C140">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="D140" t="s">
         <v>101</v>
@@ -4871,7 +4871,7 @@
         <v>0.9</v>
       </c>
       <c r="C141">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="D141" t="s">
         <v>101</v>
@@ -4900,7 +4900,7 @@
         <v>0.5</v>
       </c>
       <c r="C142">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="D142" t="s">
         <v>102</v>
@@ -4929,7 +4929,7 @@
         <v>0.7</v>
       </c>
       <c r="C143">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="D143" t="s">
         <v>102</v>
@@ -4958,7 +4958,7 @@
         <v>0.8</v>
       </c>
       <c r="C144">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="D144" t="s">
         <v>102</v>
@@ -4987,7 +4987,7 @@
         <v>0.9</v>
       </c>
       <c r="C145">
-        <v>111</v>
+        <v>46</v>
       </c>
       <c r="D145" t="s">
         <v>102</v>
@@ -5016,7 +5016,7 @@
         <v>0.5</v>
       </c>
       <c r="C146">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="D146" t="s">
         <v>103</v>
@@ -5045,7 +5045,7 @@
         <v>0.7</v>
       </c>
       <c r="C147">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D147" t="s">
         <v>103</v>
@@ -5074,7 +5074,7 @@
         <v>0.8</v>
       </c>
       <c r="C148">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="D148" t="s">
         <v>103</v>
@@ -5103,7 +5103,7 @@
         <v>0.9</v>
       </c>
       <c r="C149">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="D149" t="s">
         <v>103</v>
@@ -5132,7 +5132,7 @@
         <v>0.5</v>
       </c>
       <c r="C150">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D150" t="s">
         <v>104</v>
@@ -5161,7 +5161,7 @@
         <v>0.7</v>
       </c>
       <c r="C151">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D151" t="s">
         <v>104</v>
@@ -5190,7 +5190,7 @@
         <v>0.8</v>
       </c>
       <c r="C152">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="D152" t="s">
         <v>104</v>
@@ -5219,7 +5219,7 @@
         <v>0.9</v>
       </c>
       <c r="C153">
-        <v>112</v>
+        <v>48</v>
       </c>
       <c r="D153" t="s">
         <v>104</v>
@@ -5248,7 +5248,7 @@
         <v>0.5</v>
       </c>
       <c r="C154">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D154" t="s">
         <v>105</v>
@@ -5277,7 +5277,7 @@
         <v>0.7</v>
       </c>
       <c r="C155">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D155" t="s">
         <v>105</v>
@@ -5306,7 +5306,7 @@
         <v>0.8</v>
       </c>
       <c r="C156">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="D156" t="s">
         <v>105</v>
@@ -5335,7 +5335,7 @@
         <v>0.9</v>
       </c>
       <c r="C157">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="D157" t="s">
         <v>105</v>
@@ -5364,7 +5364,7 @@
         <v>0.5</v>
       </c>
       <c r="C158">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D158" t="s">
         <v>106</v>
@@ -5393,7 +5393,7 @@
         <v>0.7</v>
       </c>
       <c r="C159">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D159" t="s">
         <v>106</v>
@@ -5422,7 +5422,7 @@
         <v>0.8</v>
       </c>
       <c r="C160">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="D160" t="s">
         <v>106</v>
@@ -5451,7 +5451,7 @@
         <v>0.9</v>
       </c>
       <c r="C161">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D161" t="s">
         <v>106</v>
@@ -5480,7 +5480,7 @@
         <v>0.5</v>
       </c>
       <c r="C162">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="D162" t="s">
         <v>107</v>
@@ -5509,7 +5509,7 @@
         <v>0.7</v>
       </c>
       <c r="C163">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="D163" t="s">
         <v>107</v>
@@ -5538,7 +5538,7 @@
         <v>0.8</v>
       </c>
       <c r="C164">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="D164" t="s">
         <v>107</v>
@@ -5567,7 +5567,7 @@
         <v>0.9</v>
       </c>
       <c r="C165">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D165" t="s">
         <v>107</v>
@@ -5596,7 +5596,7 @@
         <v>0.5</v>
       </c>
       <c r="C166">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D166" t="s">
         <v>108</v>
@@ -5625,7 +5625,7 @@
         <v>0.7</v>
       </c>
       <c r="C167">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="D167" t="s">
         <v>108</v>
@@ -5654,7 +5654,7 @@
         <v>0.8</v>
       </c>
       <c r="C168">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="D168" t="s">
         <v>108</v>
@@ -5683,7 +5683,7 @@
         <v>0.9</v>
       </c>
       <c r="C169">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="D169" t="s">
         <v>108</v>
@@ -5712,7 +5712,7 @@
         <v>0.5</v>
       </c>
       <c r="C170">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="D170" t="s">
         <v>109</v>
@@ -5741,7 +5741,7 @@
         <v>0.7</v>
       </c>
       <c r="C171">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="D171" t="s">
         <v>109</v>
@@ -5770,7 +5770,7 @@
         <v>0.8</v>
       </c>
       <c r="C172">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="D172" t="s">
         <v>109</v>
@@ -5799,7 +5799,7 @@
         <v>0.9</v>
       </c>
       <c r="C173">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="D173" t="s">
         <v>109</v>
@@ -5828,7 +5828,7 @@
         <v>0.5</v>
       </c>
       <c r="C174">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D174" t="s">
         <v>110</v>
@@ -5857,7 +5857,7 @@
         <v>0.7</v>
       </c>
       <c r="C175">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D175" t="s">
         <v>110</v>
@@ -5886,7 +5886,7 @@
         <v>0.8</v>
       </c>
       <c r="C176">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="D176" t="s">
         <v>110</v>
@@ -5915,7 +5915,7 @@
         <v>0.9</v>
       </c>
       <c r="C177">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="D177" t="s">
         <v>110</v>
@@ -5944,7 +5944,7 @@
         <v>0.5</v>
       </c>
       <c r="C178">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D178" t="s">
         <v>111</v>
@@ -5973,7 +5973,7 @@
         <v>0.7</v>
       </c>
       <c r="C179">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="D179" t="s">
         <v>111</v>
@@ -6002,7 +6002,7 @@
         <v>0.8</v>
       </c>
       <c r="C180">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="D180" t="s">
         <v>111</v>
@@ -6031,7 +6031,7 @@
         <v>0.9</v>
       </c>
       <c r="C181">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="D181" t="s">
         <v>111</v>
@@ -6060,7 +6060,7 @@
         <v>0.5</v>
       </c>
       <c r="C182">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D182" t="s">
         <v>112</v>
@@ -6089,7 +6089,7 @@
         <v>0.7</v>
       </c>
       <c r="C183">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D183" t="s">
         <v>112</v>
@@ -6118,7 +6118,7 @@
         <v>0.8</v>
       </c>
       <c r="C184">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="D184" t="s">
         <v>112</v>
@@ -6147,7 +6147,7 @@
         <v>0.9</v>
       </c>
       <c r="C185">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="D185" t="s">
         <v>112</v>
@@ -6176,7 +6176,7 @@
         <v>0.5</v>
       </c>
       <c r="C186">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D186" t="s">
         <v>113</v>
@@ -6205,7 +6205,7 @@
         <v>0.7</v>
       </c>
       <c r="C187">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D187" t="s">
         <v>113</v>
@@ -6234,7 +6234,7 @@
         <v>0.8</v>
       </c>
       <c r="C188">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="D188" t="s">
         <v>113</v>
@@ -6263,7 +6263,7 @@
         <v>0.9</v>
       </c>
       <c r="C189">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="D189" t="s">
         <v>113</v>
@@ -6292,7 +6292,7 @@
         <v>0.5</v>
       </c>
       <c r="C190">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="D190" t="s">
         <v>114</v>
@@ -6321,7 +6321,7 @@
         <v>0.7</v>
       </c>
       <c r="C191">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="D191" t="s">
         <v>114</v>
@@ -6350,7 +6350,7 @@
         <v>0.8</v>
       </c>
       <c r="C192">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="D192" t="s">
         <v>114</v>
@@ -6379,7 +6379,7 @@
         <v>0.9</v>
       </c>
       <c r="C193">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="D193" t="s">
         <v>114</v>
@@ -6408,7 +6408,7 @@
         <v>0.5</v>
       </c>
       <c r="C194">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D194" t="s">
         <v>115</v>
@@ -6437,7 +6437,7 @@
         <v>0.7</v>
       </c>
       <c r="C195">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D195" t="s">
         <v>115</v>
@@ -6466,7 +6466,7 @@
         <v>0.8</v>
       </c>
       <c r="C196">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="D196" t="s">
         <v>115</v>
@@ -6495,7 +6495,7 @@
         <v>0.9</v>
       </c>
       <c r="C197">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="D197" t="s">
         <v>115</v>
@@ -6524,7 +6524,7 @@
         <v>0.5</v>
       </c>
       <c r="C198">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="D198" t="s">
         <v>116</v>
@@ -6553,7 +6553,7 @@
         <v>0.7</v>
       </c>
       <c r="C199">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="D199" t="s">
         <v>116</v>
@@ -6582,7 +6582,7 @@
         <v>0.8</v>
       </c>
       <c r="C200">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="D200" t="s">
         <v>116</v>
@@ -6611,7 +6611,7 @@
         <v>0.9</v>
       </c>
       <c r="C201">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="D201" t="s">
         <v>116</v>
@@ -6640,7 +6640,7 @@
         <v>0.5</v>
       </c>
       <c r="C202">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D202" t="s">
         <v>117</v>
@@ -6669,7 +6669,7 @@
         <v>0.7</v>
       </c>
       <c r="C203">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D203" t="s">
         <v>117</v>
@@ -6698,7 +6698,7 @@
         <v>0.8</v>
       </c>
       <c r="C204">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="D204" t="s">
         <v>117</v>
@@ -6727,7 +6727,7 @@
         <v>0.9</v>
       </c>
       <c r="C205">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D205" t="s">
         <v>117</v>
@@ -6756,7 +6756,7 @@
         <v>0.5</v>
       </c>
       <c r="C206">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="D206" t="s">
         <v>118</v>
@@ -6785,7 +6785,7 @@
         <v>0.7</v>
       </c>
       <c r="C207">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="D207" t="s">
         <v>118</v>
@@ -6814,7 +6814,7 @@
         <v>0.8</v>
       </c>
       <c r="C208">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D208" t="s">
         <v>118</v>
@@ -6843,7 +6843,7 @@
         <v>0.9</v>
       </c>
       <c r="C209">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="D209" t="s">
         <v>118</v>
@@ -6872,7 +6872,7 @@
         <v>0.5</v>
       </c>
       <c r="C210">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="D210" t="s">
         <v>119</v>
@@ -6901,7 +6901,7 @@
         <v>0.7</v>
       </c>
       <c r="C211">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="D211" t="s">
         <v>119</v>
@@ -6930,7 +6930,7 @@
         <v>0.8</v>
       </c>
       <c r="C212">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D212" t="s">
         <v>119</v>
@@ -6959,7 +6959,7 @@
         <v>0.9</v>
       </c>
       <c r="C213">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D213" t="s">
         <v>119</v>
@@ -6988,7 +6988,7 @@
         <v>0.5</v>
       </c>
       <c r="C214">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D214" t="s">
         <v>120</v>
@@ -7017,7 +7017,7 @@
         <v>0.7</v>
       </c>
       <c r="C215">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D215" t="s">
         <v>120</v>
@@ -7046,7 +7046,7 @@
         <v>0.8</v>
       </c>
       <c r="C216">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D216" t="s">
         <v>120</v>
@@ -7075,7 +7075,7 @@
         <v>0.9</v>
       </c>
       <c r="C217">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="D217" t="s">
         <v>120</v>
@@ -7104,7 +7104,7 @@
         <v>0.5</v>
       </c>
       <c r="C218">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="D218" t="s">
         <v>121</v>
@@ -7133,7 +7133,7 @@
         <v>0.7</v>
       </c>
       <c r="C219">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="D219" t="s">
         <v>121</v>
@@ -7162,7 +7162,7 @@
         <v>0.8</v>
       </c>
       <c r="C220">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="D220" t="s">
         <v>121</v>
@@ -7191,7 +7191,7 @@
         <v>0.9</v>
       </c>
       <c r="C221">
-        <v>122</v>
+        <v>63</v>
       </c>
       <c r="D221" t="s">
         <v>121</v>
@@ -7220,7 +7220,7 @@
         <v>0.5</v>
       </c>
       <c r="C222">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D222" t="s">
         <v>122</v>
@@ -7249,7 +7249,7 @@
         <v>0.7</v>
       </c>
       <c r="C223">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D223" t="s">
         <v>122</v>
@@ -7278,7 +7278,7 @@
         <v>0.8</v>
       </c>
       <c r="C224">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D224" t="s">
         <v>122</v>
@@ -7307,7 +7307,7 @@
         <v>0.9</v>
       </c>
       <c r="C225">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="D225" t="s">
         <v>122</v>
@@ -7336,7 +7336,7 @@
         <v>0.5</v>
       </c>
       <c r="C226">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D226" t="s">
         <v>123</v>
@@ -7365,7 +7365,7 @@
         <v>0.7</v>
       </c>
       <c r="C227">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="D227" t="s">
         <v>123</v>
@@ -7394,7 +7394,7 @@
         <v>0.8</v>
       </c>
       <c r="C228">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="D228" t="s">
         <v>123</v>
@@ -7423,7 +7423,7 @@
         <v>0.9</v>
       </c>
       <c r="C229">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D229" t="s">
         <v>123</v>
@@ -7452,7 +7452,7 @@
         <v>0.5</v>
       </c>
       <c r="C230">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="D230" t="s">
         <v>124</v>
@@ -7481,7 +7481,7 @@
         <v>0.7</v>
       </c>
       <c r="C231">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D231" t="s">
         <v>124</v>
@@ -7510,7 +7510,7 @@
         <v>0.8</v>
       </c>
       <c r="C232">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="D232" t="s">
         <v>124</v>
@@ -7539,7 +7539,7 @@
         <v>0.9</v>
       </c>
       <c r="C233">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="D233" t="s">
         <v>124</v>

</xml_diff>